<commit_message>
Ultimos cambios similitud y verificacion de direccion ADD: readme
</commit_message>
<xml_diff>
--- a/empresas.xlsx
+++ b/empresas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">rut</t>
   </si>
@@ -50,18 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">XIII REGION METROPOLITANA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87657500-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACEVEDO Y CIA. LTDA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">santa adela 10180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maipu</t>
   </si>
 </sst>
 </file>
@@ -295,10 +283,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,23 +325,6 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>